<commit_message>
Day end commit > 21/09
</commit_message>
<xml_diff>
--- a/rrd/AppData/Leads_Allocation.xlsx
+++ b/rrd/AppData/Leads_Allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C91657-6E1E-44EF-ADEC-9D6C185600F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38D801E-4524-4221-BACD-30BABCEA3DAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Allocation_config1" sheetId="28" r:id="rId1"/>
@@ -25,7 +25,11 @@
     <sheet name="LeadFields_TC10_2" sheetId="40" r:id="rId10"/>
     <sheet name="LeadFields_TC11_1" sheetId="41" r:id="rId11"/>
     <sheet name="LeadFields_TC11_2" sheetId="44" r:id="rId12"/>
-    <sheet name="ChangeOwner_SECURITY" sheetId="36" r:id="rId13"/>
+    <sheet name="LeadFields_TC12_1" sheetId="45" r:id="rId13"/>
+    <sheet name="LeadFields_TC12_2" sheetId="46" r:id="rId14"/>
+    <sheet name="LeadFields_TC13_1" sheetId="47" r:id="rId15"/>
+    <sheet name="LeadFields_TC13_2" sheetId="48" r:id="rId16"/>
+    <sheet name="ChangeOwner_SECURITY" sheetId="36" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="77">
   <si>
     <t>ExpectedResult</t>
   </si>
@@ -226,6 +230,48 @@
   </si>
   <si>
     <t>Automation_TC11_1</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Warm</t>
+  </si>
+  <si>
+    <t>Automation_TC12_1</t>
+  </si>
+  <si>
+    <t>Automation_TC12_2</t>
+  </si>
+  <si>
+    <t>Automation_TC12_3</t>
+  </si>
+  <si>
+    <t>Automation_TC12_4</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>Automation_TC13_1</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Automation_TC13_2</t>
+  </si>
+  <si>
+    <t>Automation_TC13_3</t>
+  </si>
+  <si>
+    <t>Automation_TC13_4</t>
+  </si>
+  <si>
+    <t>Test_2</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -678,7 +724,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +858,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1015F506-1A22-4782-A8FC-D658DD49707C}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,6 +1073,436 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E7832E-6B59-47A5-8273-0231AE5A0D77}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2222</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8392B2A6-1C7C-4A7D-8ACD-6500248F76A2}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3333</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4444</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5555</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52A74C0-C165-4178-9330-99B389B902A8}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4444</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899BD93E-68CB-4B9C-B46E-3F0DF7CBD716}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3333</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4444</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5555</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026568E-F656-4E01-B684-C163CCE0000F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1775,7 +2251,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commit request => 05/10/2020
</commit_message>
<xml_diff>
--- a/rrd/AppData/Leads_Allocation.xlsx
+++ b/rrd/AppData/Leads_Allocation.xlsx
@@ -1,75 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0CCB7C-94F5-416F-A553-73533381FABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0DF4B3-C6CC-4FD4-BD6E-5EF17F858813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="41" activeTab="43" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="36" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Allocation_config1" sheetId="28" r:id="rId1"/>
     <sheet name="Lead_Allocation_config2" sheetId="29" r:id="rId2"/>
     <sheet name="Lead_Allocation_config3" sheetId="30" r:id="rId3"/>
-    <sheet name="Lead_Allocation_config4" sheetId="31" r:id="rId4"/>
-    <sheet name="LeadFields_TC08_1" sheetId="35" r:id="rId5"/>
-    <sheet name="LeadFields_TC08_2" sheetId="34" r:id="rId6"/>
-    <sheet name="LeadFields_TC09_1" sheetId="37" r:id="rId7"/>
-    <sheet name="LeadFields_TC09_2" sheetId="38" r:id="rId8"/>
-    <sheet name="LeadFields_TC10_1" sheetId="39" r:id="rId9"/>
-    <sheet name="LeadFields_TC10_2" sheetId="40" r:id="rId10"/>
-    <sheet name="LeadFields_TC11_1" sheetId="41" r:id="rId11"/>
-    <sheet name="LeadFields_TC11_2" sheetId="44" r:id="rId12"/>
-    <sheet name="LeadFields_TC12_1" sheetId="45" r:id="rId13"/>
-    <sheet name="LeadFields_TC12_2" sheetId="46" r:id="rId14"/>
-    <sheet name="LeadFields_TC13_1" sheetId="47" r:id="rId15"/>
-    <sheet name="LeadFields_TC13_2" sheetId="48" r:id="rId16"/>
-    <sheet name="LeadRBAFilters_TC09_1" sheetId="50" r:id="rId17"/>
-    <sheet name="LeadRBAFilters_TC09_2" sheetId="51" r:id="rId18"/>
-    <sheet name="LeadRBAFilters_TC10_1" sheetId="52" r:id="rId19"/>
-    <sheet name="LeadRBAFilters_TC10_2" sheetId="53" r:id="rId20"/>
-    <sheet name="LeadRBAFilters_TC11_1" sheetId="54" r:id="rId21"/>
-    <sheet name="LeadRBAFilters_TC11_2" sheetId="55" r:id="rId22"/>
-    <sheet name="LeadRBAFilters_TC12_1" sheetId="57" r:id="rId23"/>
-    <sheet name="LeadRBAFilters_TC12_2" sheetId="59" r:id="rId24"/>
-    <sheet name="LeadRBAFilters_TC13_1" sheetId="60" r:id="rId25"/>
-    <sheet name="LeadRBAFilters_TC13_2" sheetId="61" r:id="rId26"/>
-    <sheet name="LeadRBAFilters_TC14_1" sheetId="62" r:id="rId27"/>
-    <sheet name="LeadRBAFilters_TC14_2" sheetId="63" r:id="rId28"/>
-    <sheet name="ExistingOpportunity_TC05" sheetId="71" r:id="rId29"/>
-    <sheet name="ExistingOpportunity_TC06" sheetId="65" r:id="rId30"/>
-    <sheet name="ExistingOpportunity_TC07" sheetId="66" r:id="rId31"/>
-    <sheet name="ExistingOpportunity_TC08" sheetId="67" r:id="rId32"/>
-    <sheet name="ExistingOpportunityFilter_TC10" sheetId="70" r:id="rId33"/>
-    <sheet name="ExistingOpportunityFilter_TC11" sheetId="72" r:id="rId34"/>
-    <sheet name="ExistingOpportunityFilter_TC12" sheetId="73" r:id="rId35"/>
-    <sheet name="ExistingOpportunityFilter_TC13" sheetId="74" r:id="rId36"/>
-    <sheet name="ExistingOpportunityFilter_TC14" sheetId="75" r:id="rId37"/>
-    <sheet name="ExistingOpportunityFilter_TC15" sheetId="76" r:id="rId38"/>
-    <sheet name="ExistingAccount_TC04" sheetId="78" r:id="rId39"/>
-    <sheet name="ExistingAccount_TC05" sheetId="79" r:id="rId40"/>
-    <sheet name="ExistingAccountFilter_TC08" sheetId="80" r:id="rId41"/>
-    <sheet name="ExistingAccountFilter_TC09" sheetId="81" r:id="rId42"/>
-    <sheet name="ExistingAccountFilter_TC10" sheetId="82" r:id="rId43"/>
-    <sheet name="ExistingAccountFilter_TC11" sheetId="83" r:id="rId44"/>
-    <sheet name="ChangeOwner_SECURITY" sheetId="36" r:id="rId45"/>
+    <sheet name="Lead_Allocation_config4_1" sheetId="84" r:id="rId4"/>
+    <sheet name="Lead_Allocation_config4_2" sheetId="85" r:id="rId5"/>
+    <sheet name="LeadFields_TC08_1" sheetId="35" r:id="rId6"/>
+    <sheet name="LeadFields_TC08_2" sheetId="34" r:id="rId7"/>
+    <sheet name="LeadFields_TC09_1" sheetId="37" r:id="rId8"/>
+    <sheet name="LeadFields_TC09_2" sheetId="38" r:id="rId9"/>
+    <sheet name="LeadFields_TC10_1" sheetId="39" r:id="rId10"/>
+    <sheet name="LeadFields_TC10_2" sheetId="40" r:id="rId11"/>
+    <sheet name="LeadFields_TC11_1" sheetId="41" r:id="rId12"/>
+    <sheet name="LeadFields_TC11_2" sheetId="44" r:id="rId13"/>
+    <sheet name="LeadFields_TC12_1" sheetId="45" r:id="rId14"/>
+    <sheet name="LeadFields_TC12_2" sheetId="46" r:id="rId15"/>
+    <sheet name="LeadFields_TC13_1" sheetId="47" r:id="rId16"/>
+    <sheet name="LeadFields_TC13_2" sheetId="48" r:id="rId17"/>
+    <sheet name="LeadRBAFilters_TC09_1" sheetId="50" r:id="rId18"/>
+    <sheet name="LeadRBAFilters_TC09_2" sheetId="51" r:id="rId19"/>
+    <sheet name="LeadRBAFilters_TC10_1" sheetId="52" r:id="rId20"/>
+    <sheet name="LeadRBAFilters_TC10_2" sheetId="53" r:id="rId21"/>
+    <sheet name="LeadRBAFilters_TC11_1" sheetId="54" r:id="rId22"/>
+    <sheet name="LeadRBAFilters_TC11_2" sheetId="55" r:id="rId23"/>
+    <sheet name="LeadRBAFilters_TC12_1" sheetId="57" r:id="rId24"/>
+    <sheet name="LeadRBAFilters_TC12_2" sheetId="59" r:id="rId25"/>
+    <sheet name="LeadRBAFilters_TC13_1" sheetId="60" r:id="rId26"/>
+    <sheet name="LeadRBAFilters_TC13_2" sheetId="61" r:id="rId27"/>
+    <sheet name="LeadRBAFilters_TC14_1" sheetId="62" r:id="rId28"/>
+    <sheet name="LeadRBAFilters_TC14_2" sheetId="63" r:id="rId29"/>
+    <sheet name="ExistingOpportunity_TC05" sheetId="71" r:id="rId30"/>
+    <sheet name="ExistingOpportunity_TC06" sheetId="65" r:id="rId31"/>
+    <sheet name="ExistingOpportunity_TC07" sheetId="66" r:id="rId32"/>
+    <sheet name="ExistingOpportunity_TC08" sheetId="67" r:id="rId33"/>
+    <sheet name="ExistingOpportunityFilter_TC10" sheetId="70" r:id="rId34"/>
+    <sheet name="ExistingOpportunityFilter_TC11" sheetId="72" r:id="rId35"/>
+    <sheet name="ExistingOpportunityFilter_TC12" sheetId="73" r:id="rId36"/>
+    <sheet name="ExistingOpportunityFilter_TC13" sheetId="74" r:id="rId37"/>
+    <sheet name="ExistingOpportunityFilter_TC14" sheetId="75" r:id="rId38"/>
+    <sheet name="ExistingOpportunityFilter_TC15" sheetId="76" r:id="rId39"/>
+    <sheet name="ExistingAccount_TC04" sheetId="78" r:id="rId40"/>
+    <sheet name="ExistingAccount_TC05" sheetId="79" r:id="rId41"/>
+    <sheet name="ExistingAccountFilter_TC08" sheetId="80" r:id="rId42"/>
+    <sheet name="ExistingAccountFilter_TC09" sheetId="81" r:id="rId43"/>
+    <sheet name="ExistingAccountFilter_TC10" sheetId="82" r:id="rId44"/>
+    <sheet name="ExistingAccountFilter_TC11" sheetId="83" r:id="rId45"/>
+    <sheet name="ChangeOwner_SECURITY" sheetId="36" r:id="rId46"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="173">
   <si>
     <t>ExpectedResult</t>
   </si>
@@ -582,6 +591,12 @@
   </si>
   <si>
     <t>MIR_TC11_2</t>
+  </si>
+  <si>
+    <t>Expectedwhilecreation</t>
+  </si>
+  <si>
+    <t>Round Robin Queue</t>
   </si>
 </sst>
 </file>
@@ -1036,6 +1051,91 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67F7874-C494-4789-ACBB-3EDC1C765EF9}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2222</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D91B1D1-A801-446A-B01F-6EFDA5A065E9}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -1169,7 +1269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFFE4C9-30A6-4E2A-8AE4-F98ADFF84ADB}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1254,7 +1354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1015F506-1A22-4782-A8FC-D658DD49707C}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -1388,7 +1488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E7832E-6B59-47A5-8273-0231AE5A0D77}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1470,7 +1570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8392B2A6-1C7C-4A7D-8ACD-6500248F76A2}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -1603,7 +1703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52A74C0-C165-4178-9330-99B389B902A8}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1686,7 +1786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899BD93E-68CB-4B9C-B46E-3F0DF7CBD716}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -1818,7 +1918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE4962B-B33D-4849-8F5F-2A9293C013C6}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1896,7 +1996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545FA56A-D5C6-4A29-A919-40951A0E50EC}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -2012,92 +2112,6 @@
       <c r="G4" t="s">
         <v>5</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5B3458-9FF9-4F5E-AA6D-7F0EEF1BCF27}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1111</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2218,6 +2232,92 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5B3458-9FF9-4F5E-AA6D-7F0EEF1BCF27}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1111</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C017F951-99ED-4487-BD5D-7FA58D6556A0}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -2324,7 +2424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08D94CE-CEAF-4FF2-A3AF-19BD4B339255}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -2406,7 +2506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6246F98-8A3F-41F5-BEB5-98AE1BF4B69C}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -2540,7 +2640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8435E02E-D9B0-44B0-956F-3934ECFF3A0C}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -2622,7 +2722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885BD5FD-775E-4F4F-85B2-AD19F773653A}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -2754,7 +2854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D9B797-D14E-4A88-9079-37A8B7A53928}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -2836,7 +2936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8591945-C705-48B1-A81B-7C623DB0B0E6}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -2967,7 +3067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5F1562-864B-485F-BF8E-1E241BAB6C0E}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -3042,7 +3142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A90C40A-A7C1-48DD-8DE1-C6DBD425FC00}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -3159,107 +3259,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E14A3A-7394-4364-B237-8F772F062935}">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3333</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4444</v>
-      </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3378,6 +3377,107 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E14A3A-7394-4364-B237-8F772F062935}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3333</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4444</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875345C0-23D4-4B8F-B0F2-773BCB5578C9}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -3485,7 +3585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321A2401-A4C8-4477-A64C-0BDBE390DA8E}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -3584,7 +3684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0488F364-BD3E-4042-AB85-F9AC4BF5E7CA}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -3709,7 +3809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EEF60B-D821-44C9-98FD-C0CBBCC1E324}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -3785,7 +3885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117EDB5A-6D56-4BB4-80F8-EBBFDCDACA70}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -3893,7 +3993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB03C74-9E59-47B2-8BCB-40735B12FB12}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -4010,11 +4110,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E237F24C-FF7C-44FD-8F07-4F23E7951388}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4165,7 +4267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1059F17F-EC2D-4453-BE54-DD88A5A21975}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -4272,7 +4374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84027167-E060-4BCD-ABEE-8FD78FD6BCDB}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -4391,7 +4493,93 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B5FD4A-4030-4AA6-93ED-6FC0A45E5798}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1111</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6C4C29-051F-4D87-853D-1CB326BD98DC}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -4466,120 +4654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025F2540-DF6E-49A0-A9F3-985CF2F6200A}">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11111110</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>22222200</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FCE50B-6A07-4700-8F04-C59FFEA040C5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -4655,7 +4730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AD505C-BE2A-4506-99EB-B480F483ABC1}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -4785,7 +4860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BFB428-8133-4CA0-AF75-9D75E2BB4791}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -4905,7 +4980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A281D81-2BC4-47AA-8C30-BCF14BA56F5B}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -5036,11 +5111,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673BC398-92F0-4EAF-A016-39E6441387B0}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -5173,7 +5248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026568E-F656-4E01-B684-C163CCE0000F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -5203,6 +5278,95 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233A2E8F-992D-4CFF-8551-CC94A0F6D4F3}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF86BD47-CAAE-4F99-A68B-49CB8D2C32C0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -5279,7 +5443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC74BFFA-765D-43AC-9A42-CBDFB61BFFB6}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -5381,7 +5545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2A0134-9C74-4651-8895-EF3B56FCB201}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -5467,7 +5631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B771A1D5-426E-4A6C-BDD3-2918F60121CA}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -5576,89 +5740,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67F7874-C494-4789-ACBB-3EDC1C765EF9}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2222</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>